<commit_message>
support read entity at specific sheetName
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/books.xlsx
+++ b/src/test/resources/xlsx/books.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walter/project/xlsx-reader/src/test/resources/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95576CBE-0536-E34F-9049-8B9BFB77EFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14480B18-1631-384D-A892-9A1ABC825E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="760" windowWidth="28240" windowHeight="17340" xr2:uid="{45A2433F-DDF2-D84F-B32C-D21A8E47DC33}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" activeTab="1" xr2:uid="{45A2433F-DDF2-D84F-B32C-D21A8E47DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="76">
   <si>
     <t>BOOKS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -442,12 +443,48 @@
     <t>[明] 罗贯中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF3377AA"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>曹雪芹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF3377AA"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF3377AA"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>著</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J.K.罗琳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -539,6 +576,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF3377AA"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -586,7 +630,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,14 +655,17 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -937,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C85D40-16BE-6649-A109-04658BC31D88}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="118" workbookViewId="0">
+      <selection sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -955,15 +1002,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="27">
       <c r="A2" s="7" t="s">
@@ -995,10 +1042,10 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>63</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1230,4 +1277,298 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A05FA89-AA38-BA43-B186-1792A46490AA}">
+  <dimension ref="I20:O31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="10" max="10" width="31.1640625" customWidth="1"/>
+    <col min="11" max="11" width="44.83203125" customWidth="1"/>
+    <col min="12" max="12" width="35.33203125" customWidth="1"/>
+    <col min="15" max="15" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="20" spans="9:15" ht="26">
+      <c r="I20" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="21" spans="9:15" ht="27">
+      <c r="I21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="9:15" ht="33">
+      <c r="I22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="9:15" ht="19">
+      <c r="I23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="9:15" ht="38">
+      <c r="I24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="9:15" ht="38">
+      <c r="I25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="9:15" ht="19">
+      <c r="I26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="9:15" ht="38">
+      <c r="I27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="9:15" ht="38">
+      <c r="I28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="9:15" ht="38">
+      <c r="I29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="9:15" ht="38">
+      <c r="I30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="9:15" ht="19">
+      <c r="I31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I20:O20"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M22" r:id="rId1" display="https://book.douban.com/press/2287" xr:uid="{CFE2ED07-66F3-1542-A4E9-0BB5AB9A858D}"/>
+    <hyperlink ref="K23" r:id="rId2" display="https://book.douban.com/author/4503668" xr:uid="{239E9351-861F-2341-BDDD-CF03701AF9BE}"/>
+    <hyperlink ref="K26" r:id="rId3" display="https://book.douban.com/search/%E5%88%98%E6%85%88%E6%AC%A3" xr:uid="{746AA726-34E1-7D4A-8819-9762235A19C1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>